<commit_message>
guías de uso PAUA
</commit_message>
<xml_diff>
--- a/PAUA/16 GUIAS DE USUARIOS/Mattriz guias.xlsx
+++ b/PAUA/16 GUIAS DE USUARIOS/Mattriz guias.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github Repositorio\All-documents\PAUA\16 GUIAS DE USUARIOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\github\All-documents\PAUA\16 GUIAS DE USUARIOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="14">
   <si>
     <t>USUARIOS</t>
   </si>
@@ -57,6 +57,15 @@
   </si>
   <si>
     <t>ADMINISTRACION DE AYUDAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GUÍAS DE USO </t>
+  </si>
+  <si>
+    <t>MATRIZ DE GUÍAS PAUA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VIDEOS </t>
   </si>
 </sst>
 </file>
@@ -130,7 +139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -147,6 +156,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -428,91 +443,156 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:D10"/>
+  <dimension ref="C1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C1" sqref="C1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="52.28515625" customWidth="1"/>
-    <col min="4" max="4" width="53.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="52.28515625" customWidth="1"/>
+    <col min="6" max="6" width="53.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C2" s="5" t="s">
+    <row r="1" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+    </row>
+    <row r="2" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5"/>
-    </row>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C4" s="3" t="s">
+      <c r="E4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C2:D2"/>
+  <mergeCells count="2">
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
guías de usuario aportaciones estatales
</commit_message>
<xml_diff>
--- a/PAUA/16 GUIAS DE USUARIOS/Mattriz guias.xlsx
+++ b/PAUA/16 GUIAS DE USUARIOS/Mattriz guias.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="15">
   <si>
     <t>USUARIOS</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t xml:space="preserve">VIDEOS </t>
+  </si>
+  <si>
+    <t>n/a</t>
   </si>
 </sst>
 </file>
@@ -445,8 +448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,7 +572,7 @@
         <v>8</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>8</v>
@@ -583,7 +586,7 @@
         <v>8</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>8</v>

</xml_diff>